<commit_message>
some list manupulation is added
</commit_message>
<xml_diff>
--- a/dataanalysis.xlsx
+++ b/dataanalysis.xlsx
@@ -16,9 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>1.line</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve"> day</t>
+  </si>
+  <si>
+    <t>type of book</t>
+  </si>
+  <si>
+    <t>number of page</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>self</t>
   </si>
 </sst>
 </file>
@@ -350,17 +365,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>